<commit_message>
small update after running to check that moving functions to utils did not break anything
</commit_message>
<xml_diff>
--- a/output_graphs/house_cp_gini_table.xlsx
+++ b/output_graphs/house_cp_gini_table.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1781,35 +1781,35 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[59, 343]</t>
+          <t>[57, 343]</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.353234</v>
+        <v>0.3575</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[1, 192, 1, 208]</t>
+          <t>[1, 190, 1, 208]</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0.504975</v>
+        <v>0.50625</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[2, 6, 4, 12, 45, 9, 7, 1, 26, 13, 1, 2, 5, 3, 16, 8, 4, 7, 7, 9, 7, 4, 12, 8, 9, 4, 3, 7, 1, 5, 1, 7, 2, 5, 19, 13, 5, 8, 17, 1, 8, 1, 9, 34, 3, 4, 1, 8, 7, 1, 1]</t>
+          <t>[2, 6, 4, 12, 45, 9, 7, 1, 26, 13, 1, 2, 5, 3, 16, 8, 4, 7, 7, 9, 7, 4, 12, 8, 9, 4, 3, 7, 1, 3, 1, 7, 2, 5, 19, 13, 5, 8, 17, 1, 8, 1, 9, 34, 3, 4, 1, 8, 7, 1, 1]</t>
         </is>
       </c>
       <c r="G35" s="2" t="n">
-        <v>0.476149</v>
+        <v>0.48</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>[1, 90, 1, 184, 118, 2, 4, 1, 1]</t>
+          <t>[1, 90, 1, 182, 118, 2, 4, 1, 1]</t>
         </is>
       </c>
       <c r="I35" s="2" t="n">
-        <v>0.698729</v>
+        <v>0.697778</v>
       </c>
     </row>
     <row r="36">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[3, 0]</t>
+          <t>[4, 0]</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[0, 3, 0, 0]</t>
+          <t>[0, 0, 0, 4]</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
@@ -1875,15 +1875,15 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="G37" s="2" t="n">
-        <v>0.980392</v>
+        <v>0.970588</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 3, 0, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0, 4, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="I37" s="2" t="n">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 3]</t>
+          <t>[0, 3, 0, 0]</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
@@ -1953,7 +1953,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0, 0, 3, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="G39" s="2" t="n">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 2]</t>
+          <t>[0, 2, 0, 0]</t>
         </is>
       </c>
       <c r="E44" s="2" t="n">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 2, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 2, 0, 0, 0, 0]</t>
+          <t>[0, 0, 0, 2, 0, 0, 0, 0, 0]</t>
         </is>
       </c>
       <c r="I44" s="2" t="n">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[0, 1, 0, 0]</t>
+          <t>[0, 0, 0, 1]</t>
         </is>
       </c>
       <c r="E52" s="2" t="n">
@@ -2460,18 +2460,57 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>0.980392</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 1, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="I52" s="2" t="n">
+        <v>0.888889</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Asynchronous label propagation  community 18</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>[1, 0]</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>[0, 1, 0, 0]</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
           <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0]</t>
         </is>
       </c>
-      <c r="G52" s="2" t="n">
-        <v>0.980392</v>
-      </c>
-      <c r="H52" t="inlineStr">
+      <c r="G53" s="2" t="n">
+        <v>0.980392</v>
+      </c>
+      <c r="H53" t="inlineStr">
         <is>
           <t>[0, 0, 0, 0, 1, 0, 0, 0, 0]</t>
         </is>
       </c>
-      <c r="I52" s="2" t="n">
+      <c r="I53" s="2" t="n">
         <v>0.888889</v>
       </c>
     </row>

</xml_diff>